<commit_message>
them 2 mau cau: số lần tăng, tăng liên tục
</commit_message>
<xml_diff>
--- a/du_lieu_btl.xlsx
+++ b/du_lieu_btl.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14794" windowHeight="5162"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14794" windowHeight="5162" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="VN-INDEX" sheetId="2" r:id="rId1"/>
@@ -3282,8 +3282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -4118,7 +4118,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -5717,7 +5717,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>